<commit_message>
Helper table for poke correlation calculation
</commit_message>
<xml_diff>
--- a/Data Analysis/oxy self admin.xlsx
+++ b/Data Analysis/oxy self admin.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atanugiri/Downloads/Record Paper/Data-Analysis/Data Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBFF37E-B883-42A5-9A43-34D01E7D6835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9729D553-82A5-AA49-9617-0AD260BC04B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDE23E3B-0D2F-4810-B26E-6D8B86FE8C66}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CDE23E3B-0D2F-4810-B26E-6D8B86FE8C66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Captain</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Wanda</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>Woody</t>
+  </si>
+  <si>
+    <t>Trixie</t>
   </si>
 </sst>
 </file>
@@ -420,20 +432,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C281FED-6FEC-4CCD-8B02-532E924E6C8C}">
-  <dimension ref="D2:R17"/>
+  <dimension ref="D2:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:18" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:18" x14ac:dyDescent="0.2">
       <c r="E3">
         <v>1</v>
       </c>
@@ -477,17 +489,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>3</v>
       </c>
       <c r="E7">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F7">
         <v>31</v>
@@ -529,12 +541,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8">
         <v>21</v>
@@ -576,12 +588,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F9">
         <v>17</v>
@@ -623,12 +635,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="F10">
         <v>54</v>
@@ -670,12 +682,12 @@
         <v>514</v>
       </c>
     </row>
-    <row r="11" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>2</v>
       </c>
       <c r="E11">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F11">
         <v>26</v>
@@ -717,12 +729,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>4</v>
       </c>
       <c r="E12">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12">
         <v>17</v>
@@ -764,12 +776,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F13">
         <v>11</v>
@@ -811,12 +823,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>10</v>
       </c>
       <c r="E14">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>59</v>
@@ -858,8 +870,149 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" t="s">
+    <row r="15" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>36</v>
+      </c>
+      <c r="I15">
+        <v>40</v>
+      </c>
+      <c r="J15">
+        <v>66</v>
+      </c>
+      <c r="K15">
+        <v>32</v>
+      </c>
+      <c r="L15">
+        <v>107</v>
+      </c>
+      <c r="M15">
+        <v>77</v>
+      </c>
+      <c r="N15" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P15" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q15">
+        <v>21</v>
+      </c>
+      <c r="R15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16">
+        <v>31</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>9</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16">
+        <v>14</v>
+      </c>
+      <c r="K16">
+        <v>14</v>
+      </c>
+      <c r="L16">
+        <v>14</v>
+      </c>
+      <c r="M16">
+        <v>10</v>
+      </c>
+      <c r="N16">
+        <v>9</v>
+      </c>
+      <c r="O16">
+        <v>10</v>
+      </c>
+      <c r="P16">
+        <v>23.5</v>
+      </c>
+      <c r="Q16">
+        <v>37</v>
+      </c>
+      <c r="R16">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>21</v>
+      </c>
+      <c r="F17">
+        <v>17.5</v>
+      </c>
+      <c r="G17">
+        <v>14</v>
+      </c>
+      <c r="H17">
+        <v>24</v>
+      </c>
+      <c r="I17">
+        <v>23</v>
+      </c>
+      <c r="J17">
+        <v>31</v>
+      </c>
+      <c r="K17">
+        <v>7</v>
+      </c>
+      <c r="L17">
+        <v>10</v>
+      </c>
+      <c r="M17">
+        <v>8.5</v>
+      </c>
+      <c r="N17">
+        <v>7</v>
+      </c>
+      <c r="O17">
+        <v>19</v>
+      </c>
+      <c r="P17">
+        <v>17</v>
+      </c>
+      <c r="Q17">
+        <v>24</v>
+      </c>
+      <c r="R17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>